<commit_message>
Change "Prior ..." columns to "Last at ..." to make meaning clearer
</commit_message>
<xml_diff>
--- a/resources/templates/work_to_list.xlsx
+++ b/resources/templates/work_to_list.xlsx
@@ -51,18 +51,6 @@
     <t>Part Description</t>
   </si>
   <si>
-    <t>Prior Op</t>
-  </si>
-  <si>
-    <t>Prior WC No</t>
-  </si>
-  <si>
-    <t>Prior WC</t>
-  </si>
-  <si>
-    <t>Prior Production Line</t>
-  </si>
-  <si>
     <t>DBR Zone</t>
   </si>
   <si>
@@ -130,6 +118,18 @@
   </si>
   <si>
     <t>Conventional Lathes</t>
+  </si>
+  <si>
+    <t>Last at Op</t>
+  </si>
+  <si>
+    <t>Last at WC No</t>
+  </si>
+  <si>
+    <t>Last at WC</t>
+  </si>
+  <si>
+    <t>Last at Production Line</t>
   </si>
 </sst>
 </file>
@@ -249,7 +249,7 @@
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="28">
+  <dxfs count="15">
     <dxf>
       <font>
         <color theme="0"/>
@@ -332,145 +332,6 @@
         <vertical/>
         <horizontal/>
       </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor theme="1" tint="0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0" tint="-4.9989318521683403E-2"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor rgb="FFC00000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1" tint="0.34998626667073579"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0" tint="-4.9989318521683403E-2"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1" tint="0.34998626667073579"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0" tint="-4.9989318521683403E-2"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1" tint="0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <border>
-        <bottom style="thin">
-          <color theme="1" tint="0.24994659260841701"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor theme="1" tint="0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0" tint="-4.9989318521683403E-2"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor rgb="FFC00000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1" tint="0.34998626667073579"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0" tint="-4.9989318521683403E-2"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1" tint="0.34998626667073579"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0" tint="-4.9989318521683403E-2"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1" tint="0.24994659260841701"/>
-        </patternFill>
-      </fill>
     </dxf>
     <dxf>
       <border>
@@ -534,14 +395,14 @@
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="3r" pivot="0" count="8">
-      <tableStyleElement type="headerRow" dxfId="27"/>
-      <tableStyleElement type="totalRow" dxfId="26"/>
-      <tableStyleElement type="firstColumn" dxfId="25"/>
-      <tableStyleElement type="lastColumn" dxfId="24"/>
+      <tableStyleElement type="headerRow" dxfId="14"/>
+      <tableStyleElement type="totalRow" dxfId="13"/>
+      <tableStyleElement type="firstColumn" dxfId="12"/>
+      <tableStyleElement type="lastColumn" dxfId="11"/>
       <tableStyleElement type="firstRowStripe" size="3"/>
-      <tableStyleElement type="secondRowStripe" size="3" dxfId="23"/>
-      <tableStyleElement type="firstColumnStripe" dxfId="22"/>
-      <tableStyleElement type="secondColumnStripe" dxfId="21"/>
+      <tableStyleElement type="secondRowStripe" size="3" dxfId="10"/>
+      <tableStyleElement type="firstColumnStripe" dxfId="9"/>
+      <tableStyleElement type="secondColumnStripe" dxfId="8"/>
     </tableStyle>
   </tableStyles>
   <extLst>
@@ -898,7 +759,7 @@
         <v>3</v>
       </c>
       <c r="E1" s="9" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="F1" s="11" t="s">
         <v>4</v>
@@ -907,7 +768,7 @@
         <v>5</v>
       </c>
       <c r="H1" s="11" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="I1" s="11" t="s">
         <v>6</v>
@@ -919,48 +780,48 @@
         <v>8</v>
       </c>
       <c r="L1" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="M1" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="N1" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="O1" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="P1" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q1" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="M1" s="11" t="s">
+      <c r="R1" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="N1" s="11" t="s">
+      <c r="S1" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="O1" s="11" t="s">
+      <c r="T1" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="P1" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="Q1" s="11" t="s">
+      <c r="U1" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="R1" s="11" t="s">
+      <c r="V1" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="S1" s="11" t="s">
+      <c r="W1" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="T1" s="11" t="s">
+      <c r="X1" s="11" t="s">
         <v>16</v>
-      </c>
-      <c r="U1" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="V1" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="W1" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="X1" s="11" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:24" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B2" s="8">
         <v>110120130</v>
@@ -984,46 +845,46 @@
         <v>13.03</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="J2" s="2">
         <v>2</v>
       </c>
       <c r="K2" s="7" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="L2" s="2">
         <v>40</v>
       </c>
       <c r="M2" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="N2" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="O2" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="P2" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q2" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="R2" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="N2" s="7" t="s">
+      <c r="S2" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="O2" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="P2" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="Q2" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="R2" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="S2" s="2" t="s">
-        <v>30</v>
-      </c>
       <c r="T2" s="2" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="U2" s="1">
         <v>12</v>
       </c>
       <c r="V2" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="W2" s="1">
         <v>1</v>

</xml_diff>